<commit_message>
-Estado de cuentas corrientes con diferentes listas -Lista Completa -Conciliada -No Conciliada
-Vinculos para ver el voucher al que pertenece tanto en Estado de cuentas corrientes
como en Libro Mayor

-Reportes re ordenados.
</commit_message>
<xml_diff>
--- a/TryTestWeb/App_Data/ESTADOCTASCORRIENTES.xlsx
+++ b/TryTestWeb/App_Data/ESTADOCTASCORRIENTES.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GEOGEST\TryTestWeb\App_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C017CAD3-E86F-46C0-9887-1FA05D9A2388}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{356C5CB0-12DB-4B8D-A2DF-C89CD5DADE02}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,12 +25,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
     <t>ESTADO DE CUENTAS CORRIENTES</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CTA. AUXILIAR: </t>
   </si>
 </sst>
 </file>
@@ -348,7 +345,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="C8:D9"/>
+  <dimension ref="D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
@@ -362,19 +359,16 @@
     <col min="4" max="4" width="26.140625" customWidth="1"/>
     <col min="5" max="5" width="21.7109375" customWidth="1"/>
     <col min="6" max="6" width="18.5703125" customWidth="1"/>
-    <col min="7" max="7" width="12.7109375" customWidth="1"/>
+    <col min="7" max="7" width="25.140625" customWidth="1"/>
     <col min="8" max="8" width="12.85546875" customWidth="1"/>
-    <col min="9" max="9" width="11.140625" customWidth="1"/>
+    <col min="9" max="9" width="17.140625" customWidth="1"/>
+    <col min="10" max="10" width="13.5703125" customWidth="1"/>
+    <col min="11" max="11" width="17.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="8" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D8" t="s">
         <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C9" t="s">
-        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>